<commit_message>
Updates to whitelist for indicators
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="173">
   <si>
     <t>short</t>
   </si>
@@ -527,6 +527,18 @@
   </si>
   <si>
     <t>procurement</t>
+  </si>
+  <si>
+    <t>description_albanian</t>
+  </si>
+  <si>
+    <t>name_albanian</t>
+  </si>
+  <si>
+    <t>name_serbian</t>
+  </si>
+  <si>
+    <t>description_serbian</t>
   </si>
 </sst>
 </file>
@@ -575,8 +587,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -589,15 +603,17 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1404,19 +1420,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>135</v>
       </c>
@@ -1424,13 +1444,19 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>170</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>171</v>
+      </c>
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -1438,7 +1464,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -1446,7 +1472,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1454,7 +1480,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -1462,7 +1488,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -1470,7 +1496,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -1478,7 +1504,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -1486,7 +1512,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -1494,7 +1520,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -1502,7 +1528,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -1510,7 +1536,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -1518,7 +1544,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -1526,7 +1552,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -1534,7 +1560,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -1542,7 +1568,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -1715,6 +1741,7 @@
     <sortCondition ref="B3"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added new method to regenrate whitelists
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
     <sheet name="indicators" sheetId="2" r:id="rId2"/>
+    <sheet name="problems" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="173">
-  <si>
-    <t>short</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="156">
   <si>
     <t>albanian</t>
   </si>
@@ -37,9 +35,6 @@
     <t>Dragash</t>
   </si>
   <si>
-    <t>Gliogovc</t>
-  </si>
-  <si>
     <t>Drenas</t>
   </si>
   <si>
@@ -427,108 +422,6 @@
     <t>youth activities</t>
   </si>
   <si>
-    <t>original</t>
-  </si>
-  <si>
-    <t>preschool</t>
-  </si>
-  <si>
-    <t>cemetery</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>emergency</t>
-  </si>
-  <si>
-    <t>environment</t>
-  </si>
-  <si>
-    <t>family_medical</t>
-  </si>
-  <si>
-    <t>police</t>
-  </si>
-  <si>
-    <t>local_road</t>
-  </si>
-  <si>
-    <t>national_road</t>
-  </si>
-  <si>
-    <t>funds</t>
-  </si>
-  <si>
-    <t>administration</t>
-  </si>
-  <si>
-    <t>assembly</t>
-  </si>
-  <si>
-    <t>parks</t>
-  </si>
-  <si>
-    <t>nature</t>
-  </si>
-  <si>
-    <t>phone_post</t>
-  </si>
-  <si>
-    <t>tax_procedures</t>
-  </si>
-  <si>
-    <t>cultural_activities</t>
-  </si>
-  <si>
-    <t>cultural_heritage</t>
-  </si>
-  <si>
-    <t>health</t>
-  </si>
-  <si>
-    <t>lighting</t>
-  </si>
-  <si>
-    <t>transport</t>
-  </si>
-  <si>
-    <t>recruitment</t>
-  </si>
-  <si>
-    <t>sewage</t>
-  </si>
-  <si>
-    <t>social_services</t>
-  </si>
-  <si>
-    <t>sports</t>
-  </si>
-  <si>
-    <t>mayor</t>
-  </si>
-  <si>
-    <t>traffic</t>
-  </si>
-  <si>
-    <t>urban_planning</t>
-  </si>
-  <si>
-    <t>waste</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>youth</t>
-  </si>
-  <si>
-    <t>school</t>
-  </si>
-  <si>
-    <t>procurement</t>
-  </si>
-  <si>
     <t>description_albanian</t>
   </si>
   <si>
@@ -539,6 +432,63 @@
   </si>
   <si>
     <t>description_serbian</t>
+  </si>
+  <si>
+    <t>Gllogovc</t>
+  </si>
+  <si>
+    <t>albanian_name</t>
+  </si>
+  <si>
+    <t>serbian_name</t>
+  </si>
+  <si>
+    <t>Lack of economic growth</t>
+  </si>
+  <si>
+    <t>Road infrastructure</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
+  </si>
+  <si>
+    <t>Crime</t>
+  </si>
+  <si>
+    <t>Corruption</t>
+  </si>
+  <si>
+    <t>Poverty/Low standard of living</t>
+  </si>
+  <si>
+    <t>Inter-ethnic relations</t>
+  </si>
+  <si>
+    <t>Poor water supply</t>
+  </si>
+  <si>
+    <t>Environmental pollution</t>
+  </si>
+  <si>
+    <t>Lack of general or personal security</t>
+  </si>
+  <si>
+    <t>Limited freedom of movement</t>
+  </si>
+  <si>
+    <t>Poor electricity supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poorly functioning rubbish collection service </t>
+  </si>
+  <si>
+    <t>albanian_description</t>
+  </si>
+  <si>
+    <t>serbian_description</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -587,8 +537,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,17 +557,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -945,9 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -958,453 +914,453 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1420,325 +1376,325 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
         <v>135</v>
       </c>
+      <c r="D1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>124</v>
-      </c>
-      <c r="B25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>132</v>
-      </c>
-      <c r="B34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" t="s">
-        <v>166</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A1:D36">
-    <sortCondition ref="B3"/>
+  <sortState ref="A2:D14">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Converted problem slugs to lower case
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="221">
   <si>
     <t>albanian</t>
   </si>
@@ -437,21 +437,9 @@
     <t>serbian_name</t>
   </si>
   <si>
-    <t>Lack of economic growth</t>
-  </si>
-  <si>
-    <t>Road infrastructure</t>
-  </si>
-  <si>
     <t>Unemployment</t>
   </si>
   <si>
-    <t>Crime</t>
-  </si>
-  <si>
-    <t>Corruption</t>
-  </si>
-  <si>
     <t>Poverty/Low standard of living</t>
   </si>
   <si>
@@ -657,6 +645,45 @@
   </si>
   <si>
     <t>fire and emergency services</t>
+  </si>
+  <si>
+    <t>corruption</t>
+  </si>
+  <si>
+    <t>crime</t>
+  </si>
+  <si>
+    <t>environmental pollution</t>
+  </si>
+  <si>
+    <t>inter-ethnic relations</t>
+  </si>
+  <si>
+    <t>lack of economic growth</t>
+  </si>
+  <si>
+    <t>lack of general or personal security</t>
+  </si>
+  <si>
+    <t>limited freedom of movement</t>
+  </si>
+  <si>
+    <t>poor electricity supply</t>
+  </si>
+  <si>
+    <t>poor water supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poorly functioning rubbish collection service </t>
+  </si>
+  <si>
+    <t>poverty/Low standard of living</t>
+  </si>
+  <si>
+    <t>road infrastructure</t>
+  </si>
+  <si>
+    <t>unemployment</t>
   </si>
 </sst>
 </file>
@@ -705,8 +732,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -751,7 +782,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -772,6 +803,8 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -792,6 +825,8 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1134,7 +1169,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1598,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1613,7 +1648,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
         <v>132</v>
@@ -1639,10 +1674,10 @@
         <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1656,27 +1691,27 @@
         <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" t="s">
         <v>154</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>155</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1684,16 +1719,16 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" t="s">
         <v>156</v>
-      </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1707,10 +1742,10 @@
         <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1724,27 +1759,27 @@
         <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1758,10 +1793,10 @@
         <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1775,10 +1810,10 @@
         <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1792,10 +1827,10 @@
         <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1809,10 +1844,10 @@
         <v>116</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1826,10 +1861,10 @@
         <v>103</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1843,10 +1878,10 @@
         <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1860,10 +1895,10 @@
         <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1877,10 +1912,10 @@
         <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E16" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1894,10 +1929,10 @@
         <v>106</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1911,10 +1946,10 @@
         <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1928,10 +1963,10 @@
         <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E19" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1945,10 +1980,10 @@
         <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1962,10 +1997,10 @@
         <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1979,10 +2014,10 @@
         <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1996,10 +2031,10 @@
         <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2013,10 +2048,10 @@
         <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2030,10 +2065,10 @@
         <v>120</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2047,10 +2082,10 @@
         <v>121</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E26" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2064,10 +2099,10 @@
         <v>122</v>
       </c>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2081,10 +2116,10 @@
         <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E28" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2098,10 +2133,10 @@
         <v>124</v>
       </c>
       <c r="D29" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E29" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2115,10 +2150,10 @@
         <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2132,10 +2167,10 @@
         <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E31" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2149,10 +2184,10 @@
         <v>119</v>
       </c>
       <c r="D32" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E32" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2166,10 +2201,10 @@
         <v>127</v>
       </c>
       <c r="D33" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2183,10 +2218,10 @@
         <v>128</v>
       </c>
       <c r="D34" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2200,10 +2235,10 @@
         <v>129</v>
       </c>
       <c r="D35" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2217,44 +2252,44 @@
         <v>130</v>
       </c>
       <c r="D36" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E36" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C37" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E37" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E38" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2272,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2286,7 +2321,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
         <v>136</v>
@@ -2295,231 +2330,231 @@
         <v>137</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
         <v>190</v>
       </c>
-      <c r="C3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" t="s">
-        <v>194</v>
-      </c>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>219</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing up various bugs to ensure fields are dynamic
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="2"/>
@@ -11,6 +11,9 @@
     <sheet name="indicators" sheetId="2" r:id="rId2"/>
     <sheet name="problems" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicators!$A$1:$E$37</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="250">
   <si>
     <t>albanian</t>
   </si>
@@ -335,9 +338,6 @@
     <t>hospitals</t>
   </si>
   <si>
-    <t>kosovo police</t>
-  </si>
-  <si>
     <t>local road maintenance</t>
   </si>
   <si>
@@ -416,228 +416,12 @@
     <t>youth activities</t>
   </si>
   <si>
-    <t>description_albanian</t>
-  </si>
-  <si>
-    <t>name_albanian</t>
-  </si>
-  <si>
-    <t>name_serbian</t>
-  </si>
-  <si>
-    <t>description_serbian</t>
-  </si>
-  <si>
-    <t>Gllogovc</t>
-  </si>
-  <si>
-    <t>albanian_name</t>
-  </si>
-  <si>
-    <t>serbian_name</t>
-  </si>
-  <si>
-    <t>Unemployment</t>
-  </si>
-  <si>
-    <t>Poverty/Low standard of living</t>
-  </si>
-  <si>
-    <t>Inter-ethnic relations</t>
-  </si>
-  <si>
-    <t>Poor water supply</t>
-  </si>
-  <si>
-    <t>Environmental pollution</t>
-  </si>
-  <si>
-    <t>Lack of general or personal security</t>
-  </si>
-  <si>
-    <t>Limited freedom of movement</t>
-  </si>
-  <si>
-    <t>Poor electricity supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poorly functioning rubbish collection service </t>
-  </si>
-  <si>
-    <t>albanian_description</t>
-  </si>
-  <si>
-    <t>serbian_description</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
     <t>cemetery maintenance</t>
   </si>
   <si>
-    <t>cemëtery maintenancë</t>
-  </si>
-  <si>
-    <t>çultural activities</t>
-  </si>
-  <si>
-    <t>Sustainable plaid health goth pinterest YOLO, authentic hoodie hashtag fixie swag hella aesthetic banh mi fap fingerstache. Cred shoreditch godard, neutra deep v narwhal food truck flannel normcore.</t>
-  </si>
-  <si>
-    <t>Waistcoat neutra synth 90's distillery, +1 sartorial occupy pinterest ugh kickstarter.</t>
-  </si>
-  <si>
-    <t>Kombucha sartorial try-hard offal food truck. Pitchfork YOLO brooklyn stumptown locavore.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keytar swag portland, meh food truck quinoa knausgaard gastropub synth williamsburg. </t>
-  </si>
-  <si>
-    <t>Chia disrupt raw denim twee synth. Messenger bag waistcoat single-origin coffee, sartorial wolf vegan food truck. Hoodie narwhal freegan pop-up hammock hella wolf.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narwhal XOXO cardigan, seitan microdosing pabst selvage cray lo-fi skateboard brunch. </t>
-  </si>
-  <si>
-    <t>Gastropub art party sustainable, tattooed small batch vice leggings actually tote bag. Cray kinfolk hoodie mumblecore tumblr.</t>
-  </si>
-  <si>
-    <t>Cliche twee neutra bushwick, celiac photo booth distillery pitchfork selvage beard microdosing swag hoodie pinterest four dollar toast.</t>
-  </si>
-  <si>
-    <t>Ramps scenester shabby chic waistcoat food truck, four loko art party authentic.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venmo celiac kale chips, distillery stumptown offal chillwave PBR&amp;B twee cray ethical tote bag food truck. Tumblr DIY pour-over kinfolk vinyl. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fingerstache forage craft beer, intelligentsia chartreuse narwhal seitan fixie health goth paleo 3 wolf moon selvage single-origin coffee pinterest typewriter. </t>
-  </si>
-  <si>
-    <t>3 wolf moon stumptown bespoke, chillwave viral crucifix taxidermy tilde. Dreamcatcher deep v authentic, tote bag cliche shoreditch typewriter flannel disrupt.</t>
-  </si>
-  <si>
-    <t>Flank ham short loin tenderloin shoulder tail cupim porchetta boudin pork chop cow. Ham brisket pastrami salami short loin, frankfurter ribeye.</t>
-  </si>
-  <si>
-    <t>Pastrami tri-tip frankfurter venison salami, kielbasa turducken shoulder andouille jowl pig beef ribs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swine meatloaf cow sirloin, alcatra pork andouille ham t-bone prosciutto cupim turkey jowl turducken tri-tip. Salami sirloin swine chuck landjaeger jerky kielbasa hamburger jowl ground round shank cupim. </t>
-  </si>
-  <si>
-    <t>Pork belly tenderloin pork loin biltong, fatback short ribs turducken. Ham hock filet mignon drumstick andouille, turkey tenderloin corned beef landjaeger strip steak jerky.</t>
-  </si>
-  <si>
-    <t>Short ribs ribeye shank salami turkey, jerky beef ribs shoulder. Ribeye fatback ham jowl picanha meatball pig drumstick biltong andouille turkey.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tri-tip biltong flank, ball tip beef tongue tail pork chop strip steak chuck venison meatloaf jerky corned beef. </t>
-  </si>
-  <si>
-    <t>Doner prosciutto meatloaf beef. Pork chop tri-tip doner shank chuck alcatra brisket boudin jerky ribeye shoulder biltong porchetta hamburger.</t>
-  </si>
-  <si>
-    <t>T-bone chicken short ribs hamburger, salami pig jerky leberkas ham prosciutto. Kevin frankfurter kielbasa turducken turkey strip steak beef flank meatloaf landjaeger doner.</t>
-  </si>
-  <si>
-    <t>Capicola cupim hamburger ham hock ribeye t-bone shoulder pork chop cow short loin tenderloin biltong prosciutto ground round kevin.</t>
-  </si>
-  <si>
-    <t>Sausage brisket pork, pancetta leberkas fatback doner shankle pastrami swine tongue salami ground round beef ribs.</t>
-  </si>
-  <si>
-    <t>Turkey alcatra ham shank pork chop. Sirloin spare ribs beef ribs capicola, leberkas salami meatball shoulder turkey swine frankfurter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corsair American Main yo-ho-ho league ho lateen sail splice the main brace skysail pressgang fire ship. Sutler carouser galleon gally American Main Jack Ketch ye chantey yard no prey, no pay. </t>
-  </si>
-  <si>
-    <t>Gibbet killick cable Admiral of the Black league starboard loaded to the gunwalls Sail ho ahoy yawl.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured fer yer chains list chase guns maroon Davy Jones' Locker Cat o'nine tails heave to long boat rope's end execution dock. </t>
-  </si>
-  <si>
-    <t>American Main loaded to the gunwalls fire ship league clipper long boat topmast Sink me tackle cutlass. Loot come about lee coxswain gunwalls stern aye Buccaneer bilge water topmast.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red ensign Spanish Main hornswaggle warp trysail gun galleon tender scuppers hulk. Arr gun jolly boat lugsail rope's end capstan black spot clap of thunder port nipper. </t>
-  </si>
-  <si>
-    <t>Ho heave down scuttle walk the plank scallywag rutters grog blossom hang the jib Jack Tar pirate.</t>
-  </si>
-  <si>
-    <t>You know why the yankees always win, frank? it's 'cause the other teams can't stop staring at those damn pinstripes.</t>
-  </si>
-  <si>
-    <t>Two little mice fell in a bucket of cream. the first mouse quickly gave up and drowned. the second mouse, wouldn't quit. he struggled so hard that eventually he churned that cream into butter and crawled out.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Croque monsieur macaroni cheese cheesy feet. Cheesy grin fondue croque monsieur emmental cheese and wine halloumi croque monsieur cheese and wine. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fromage roquefort cheeseburger. Stinking bishop cheddar pepper jack hard cheese camembert de normandie queso edam pecorino. </t>
-  </si>
-  <si>
-    <t>Crimë</t>
-  </si>
-  <si>
-    <t>Lack of eçonomic growth</t>
-  </si>
-  <si>
-    <t>Road infrastructurë</t>
-  </si>
-  <si>
-    <t>Çorruption</t>
-  </si>
-  <si>
-    <t>Chalk and cheese bocconcini macaroni cheese rubber cheese roquefort the big cheese cheesecake dolcelatte. Cheesecake pepper jack bocconcini squirty cheese.</t>
-  </si>
-  <si>
-    <t>Gouda gouda cheese strings. Jarlsberg cheese and biscuits mozzarella squirty cheese brie cheddar manchego feta.</t>
-  </si>
-  <si>
-    <t>No wait, Doc, the bruise, the bruise on your head, I know how that happened, you told me the whole story. you were standing on your toilet and you were hanging a clock, and you fell, and you hit your head on the sink, and that's when you came up with the idea for the flux capacitor, which makes time travel possible.</t>
-  </si>
-  <si>
-    <t>About 30 years, it's a nice round number. Don't worry, I'll take care of the lightning, you take care of your pop.</t>
-  </si>
-  <si>
-    <t>By the way, what happened today, did he ask her out? Get out of town, I didn't know you did anything creative. Ah, let me read some. Who's are these?</t>
-  </si>
-  <si>
-    <t>Yeah. Well, Marty, I want to thank you for all your good advise, I'll never forget it. What's the meaning of this. Look, you gotta listen to me. Yeah but George, Lorraine wants to go with you. Give her a break.</t>
-  </si>
-  <si>
-    <t>He's your brother, Mom. The storm. Yeah, well, I still don't understand what Dad was doing in the middle of the street. Maybe you were adopted. Alright, okay Jennifer.</t>
-  </si>
-  <si>
-    <t>What if I send in the tape and they don't like it. I mean, what if they say I'm no good. What if they say, 'Get out of here, kid, you got no future.' I mean, I just don't think I can take that kind of rejection. Jesus, I'm beginning to sound like my old man.</t>
-  </si>
-  <si>
-    <t>Why is she gonna get angry with you? Calvin, why do you keep calling me Calvin? That's right. What were you doing in the middle of the street, a kid your age.</t>
-  </si>
-  <si>
-    <t>Now remember, according to my theory you interfered with with your parent's first meeting.</t>
-  </si>
-  <si>
-    <t>That's why your older brother's disappeared from that photograph. Your sister will follow and unless you repair the damages, you will be next.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">They don't mëët, they don't fall in love, they won't get married and they wont have kids. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchëgo rëd leicëster çaerphilly. Cow stinking bishop fromage frais dolcelatte red leicester cheesecake cheesy feet babybel. Caerphilly port-salut cheesy feet fondue when the cheese comes out everybody's happy goat paneer cheddar. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lo-fi kombuçha PBR&amp;B four loko williamsburg strëët art messenger bag, everyday carry literally put a bird on it meggings vice stumptown. Ethical kombucha affogato, tattooed plaid photo booth readymade. </t>
-  </si>
-  <si>
-    <t>Çhëësë slices fromage cheese on toast st. agur blue cheese cheese strings cow pepper jack lancashire. Stilton cheese triangles.</t>
-  </si>
-  <si>
     <t>representation of women</t>
   </si>
   <si>
@@ -677,13 +461,320 @@
     <t xml:space="preserve">poorly functioning rubbish collection service </t>
   </si>
   <si>
-    <t>poverty/Low standard of living</t>
-  </si>
-  <si>
     <t>road infrastructure</t>
   </si>
   <si>
     <t>unemployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Qasjen dhe cilësinë e arsimimit parashkollor</t>
+  </si>
+  <si>
+    <t>Mirëmbajtjen e varrezave</t>
+  </si>
+  <si>
+    <t>Aktivitetet e kulturës</t>
+  </si>
+  <si>
+    <t>Furnizimin me energji elektrike</t>
+  </si>
+  <si>
+    <t>Aktivitetet e emergjencës</t>
+  </si>
+  <si>
+    <t>Mbrojtjen e mjedisit</t>
+  </si>
+  <si>
+    <t>Qendrat e mjekësisë familjare</t>
+  </si>
+  <si>
+    <t>Spitalet</t>
+  </si>
+  <si>
+    <t>Mirëmbajtjen e rrugëve komunale</t>
+  </si>
+  <si>
+    <t>Mirëmbajtjen e rrugëve dhe autostradave ndërkomunale</t>
+  </si>
+  <si>
+    <t>Menaxhimin e fondeve komunale</t>
+  </si>
+  <si>
+    <t>Administratën publike</t>
+  </si>
+  <si>
+    <t>Asamblenë komunale</t>
+  </si>
+  <si>
+    <t>Parqet dhe sheshet e komunës</t>
+  </si>
+  <si>
+    <t>Brojtjen e natyrës dhe specieve</t>
+  </si>
+  <si>
+    <t>Telefoninë dhe shërbimet postare</t>
+  </si>
+  <si>
+    <t>Arsimimin fillor dhe të mesëm</t>
+  </si>
+  <si>
+    <t>Procedurat për pagesën e taksave</t>
+  </si>
+  <si>
+    <t>Mbrojtjen e trashëgimisë kulturore</t>
+  </si>
+  <si>
+    <t>Shëndetësine publike</t>
+  </si>
+  <si>
+    <t>Ndriçimin publik</t>
+  </si>
+  <si>
+    <t>Prokurimin publik/tenderët</t>
+  </si>
+  <si>
+    <t>Transportin publik</t>
+  </si>
+  <si>
+    <t>Punësimin e stafit të komunës</t>
+  </si>
+  <si>
+    <t>Përfaqësimin e minoriteteve entike në komunë</t>
+  </si>
+  <si>
+    <t>Përfaqësimin e grave në komunë</t>
+  </si>
+  <si>
+    <t>Sistemin e kanalizimit</t>
+  </si>
+  <si>
+    <t>Trotuaret</t>
+  </si>
+  <si>
+    <t>Shërbimet sociale</t>
+  </si>
+  <si>
+    <t>Aktivitetet e sportit</t>
+  </si>
+  <si>
+    <t>Kryetarin e komunës</t>
+  </si>
+  <si>
+    <t>Kontrollin dhe rregullimin e trafikut dhe parkingjeve</t>
+  </si>
+  <si>
+    <t>Planfikimin urban dhe rural</t>
+  </si>
+  <si>
+    <t>Shërbimin e mbledhjes së mbeturinave</t>
+  </si>
+  <si>
+    <t>Furnizimin me ujë</t>
+  </si>
+  <si>
+    <t>Aktivitetet e rinisë</t>
+  </si>
+  <si>
+    <t>Pristupom i kvalitetom predškolskog obrazovanja</t>
+  </si>
+  <si>
+    <t>Održavanjem groblja</t>
+  </si>
+  <si>
+    <t>Kulturnim aktivnostima</t>
+  </si>
+  <si>
+    <t>Snabdevanjem električnom energijom</t>
+  </si>
+  <si>
+    <t>Hitnim službama</t>
+  </si>
+  <si>
+    <t>Zaštitom životne sredine</t>
+  </si>
+  <si>
+    <t>Porodičnim medicinskim centrima</t>
+  </si>
+  <si>
+    <t>Bolnicama</t>
+  </si>
+  <si>
+    <t>Održavanjem lokalnih puteva</t>
+  </si>
+  <si>
+    <t>Pristupačnošću i održavanjem međuopštinskih puteva i autoputeva</t>
+  </si>
+  <si>
+    <t>Upravljanjem opštinskih fondova</t>
+  </si>
+  <si>
+    <t>Opštinskom administracijom</t>
+  </si>
+  <si>
+    <t>Opštinskom skupštinom</t>
+  </si>
+  <si>
+    <t>Opštinskim parkova i trgova</t>
+  </si>
+  <si>
+    <t>Očuvanjem prirode i vrsta</t>
+  </si>
+  <si>
+    <t>Telefonskim i poštanskim uslugama</t>
+  </si>
+  <si>
+    <t>Pristupom i kvalitetom osnovnog i srednog obrazovanja</t>
+  </si>
+  <si>
+    <t>Procedurama za plaćanje poreza</t>
+  </si>
+  <si>
+    <t>Zaštitom kulturnog nasleđa</t>
+  </si>
+  <si>
+    <t>Javnom zdravstvom</t>
+  </si>
+  <si>
+    <t>Javnom rasvetom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javnim nabavkama i tenderima
+</t>
+  </si>
+  <si>
+    <t>Javnim prevozom</t>
+  </si>
+  <si>
+    <t>Regrutovanjem opštinskog osoblja</t>
+  </si>
+  <si>
+    <t>Zastupljenost etničkih manjina u opštini</t>
+  </si>
+  <si>
+    <t>Zastupljenost žena u opštini</t>
+  </si>
+  <si>
+    <t>Kanalizacijom i sanitacijom</t>
+  </si>
+  <si>
+    <t>Trotoarima</t>
+  </si>
+  <si>
+    <t>Radom centara za socijalni rad</t>
+  </si>
+  <si>
+    <t>Sportskim aktivnostima</t>
+  </si>
+  <si>
+    <t>Gradonačelnikom</t>
+  </si>
+  <si>
+    <t>Kontrolom i regulacijom parkinga i saobraćaja</t>
+  </si>
+  <si>
+    <t>Ruralnim i urbanim planiranjem</t>
+  </si>
+  <si>
+    <t>Prikupljanjem i odlaganjem čvrstog otpada</t>
+  </si>
+  <si>
+    <t>Vodosnabdevanjem</t>
+  </si>
+  <si>
+    <t>Omladinskim aktivnostima</t>
+  </si>
+  <si>
+    <t>Korrupsioni</t>
+  </si>
+  <si>
+    <t>Krimi</t>
+  </si>
+  <si>
+    <t>Ndotja e mjedisit</t>
+  </si>
+  <si>
+    <t>Marrëdhëniet ndërt-etnike</t>
+  </si>
+  <si>
+    <t>Mungesa e rritjes ekonomike</t>
+  </si>
+  <si>
+    <t>Mungesa e sigurisë së përgjithshme dhe sigurisë personale</t>
+  </si>
+  <si>
+    <t>Liria e kufizuar e lëvizjes</t>
+  </si>
+  <si>
+    <t>Furnizimi me rryme</t>
+  </si>
+  <si>
+    <t>Furnizimi me ujë</t>
+  </si>
+  <si>
+    <t>Shërbimi i grumbullimit të mbeturinave</t>
+  </si>
+  <si>
+    <t>Varfëria/Standardi i ulët i jetesës</t>
+  </si>
+  <si>
+    <t>Infrastruktura rrugore</t>
+  </si>
+  <si>
+    <t>Papunësia</t>
+  </si>
+  <si>
+    <t>Korupcija</t>
+  </si>
+  <si>
+    <t>Kriminal</t>
+  </si>
+  <si>
+    <t>Zagađenje životne sredine</t>
+  </si>
+  <si>
+    <t>Međuetnički odnosi</t>
+  </si>
+  <si>
+    <t>Nedostatak privrednog rasta</t>
+  </si>
+  <si>
+    <t>Nedostatak opšte i lične sigurnosti</t>
+  </si>
+  <si>
+    <t>Ograničena sloboda kretanja</t>
+  </si>
+  <si>
+    <t>Loše snabdevanje električnom energijom</t>
+  </si>
+  <si>
+    <t>Loše snabdevanje vodom</t>
+  </si>
+  <si>
+    <t>Slabo funkcionisanje službe za skupljanje smeča</t>
+  </si>
+  <si>
+    <t>Siromaštvo / Nizak životni standard</t>
+  </si>
+  <si>
+    <t>Putna infrastruktura</t>
+  </si>
+  <si>
+    <t>Nezaposlenost</t>
+  </si>
+  <si>
+    <t>Gllogoc</t>
+  </si>
+  <si>
+    <t>albanian_desc</t>
+  </si>
+  <si>
+    <t>serbian_desc</t>
+  </si>
+  <si>
+    <t>poverty/low standard of living</t>
   </si>
 </sst>
 </file>
@@ -732,7 +823,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -778,11 +869,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -805,6 +908,9 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -827,6 +933,9 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1158,7 +1267,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1169,7 +1280,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1202,7 +1313,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1631,410 +1742,410 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>150</v>
       </c>
-      <c r="B4" t="s">
-        <v>151</v>
-      </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>195</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>198</v>
       </c>
       <c r="D16" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="D23" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="E23" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2042,257 +2153,245 @@
         <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>207</v>
       </c>
       <c r="D25" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="E25" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="D26" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="E26" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>209</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>210</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="E29" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>176</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="E35" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="D36" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>203</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>206</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>205</v>
-      </c>
-      <c r="B38" t="s">
-        <v>205</v>
-      </c>
-      <c r="C38" t="s">
-        <v>205</v>
-      </c>
-      <c r="D38" t="s">
-        <v>177</v>
-      </c>
-      <c r="E38" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E37">
+    <sortState ref="A2:E38">
+      <sortCondition ref="A4"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2308,258 +2407,259 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" t="s">
-        <v>189</v>
+        <v>220</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
+        <v>221</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
+        <v>222</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" t="s">
-        <v>140</v>
+        <v>223</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
+        <v>224</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" t="s">
-        <v>141</v>
+        <v>228</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>229</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" t="s">
-        <v>139</v>
+        <v>230</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
-      </c>
-      <c r="C13" t="s">
-        <v>188</v>
+        <v>231</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>200</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" t="s">
-        <v>138</v>
+        <v>232</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="D14" t="s">
-        <v>200</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D14">
-    <sortCondition ref="A2"/>
+  <sortState ref="A16:A37">
+    <sortCondition ref="A16"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Fixed some incorrect municipality translations
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicators!$A$1:$E$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">municipalities!$A$1:$C$41</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="249">
   <si>
     <t>albanian</t>
   </si>
@@ -92,9 +93,6 @@
     <t>Kamenice</t>
   </si>
   <si>
-    <t>Kosovska Kamenica</t>
-  </si>
-  <si>
     <t>Kline</t>
   </si>
   <si>
@@ -125,16 +123,7 @@
     <t>Mitrovica</t>
   </si>
   <si>
-    <t>Kosovska Mitrovica</t>
-  </si>
-  <si>
     <t>Mitrovica North</t>
-  </si>
-  <si>
-    <t>Mitrovica Veriore</t>
-  </si>
-  <si>
-    <t>Severna Kosovska Mitrovica</t>
   </si>
   <si>
     <t>Mitrovica South</t>
@@ -775,6 +764,15 @@
   </si>
   <si>
     <t>poverty/low standard of living</t>
+  </si>
+  <si>
+    <t>Severna Mitrovica</t>
+  </si>
+  <si>
+    <t>Kamenica</t>
+  </si>
+  <si>
+    <t>Mitrovicës Veriore</t>
   </si>
 </sst>
 </file>
@@ -823,8 +821,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -885,7 +891,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -911,6 +917,10 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -936,6 +946,10 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1267,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1280,7 +1294,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1294,10 +1308,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1308,62 +1322,62 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1371,10 +1385,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1415,10 +1429,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1426,307 +1440,307 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1773,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1768,622 +1782,622 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C22" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C25" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C26" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C33" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D33" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C34" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E34" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C36" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C37" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2406,7 +2420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -2421,7 +2435,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2430,231 +2444,231 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to whitelist and downloads
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="problems" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicators!$A$1:$E$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicators!$A$1:$I$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">municipalities!$A$1:$C$41</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="253">
   <si>
     <t>albanian</t>
   </si>
@@ -773,6 +773,18 @@
   </si>
   <si>
     <t>Mitrovicës Veriore</t>
+  </si>
+  <si>
+    <t>english_short</t>
+  </si>
+  <si>
+    <t>albanian_short</t>
+  </si>
+  <si>
+    <t>serbian_short</t>
+  </si>
+  <si>
+    <t>english_desc</t>
   </si>
 </sst>
 </file>
@@ -1281,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1756,652 +1768,668 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>126</v>
       </c>
       <c r="B1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>144</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>180</v>
       </c>
-      <c r="D2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="H2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>145</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>181</v>
       </c>
-      <c r="D3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="H3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>146</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>182</v>
       </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="H4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>147</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>183</v>
       </c>
-      <c r="D5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="H5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>148</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>184</v>
       </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="H6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>149</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>185</v>
       </c>
-      <c r="D7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="H7" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>130</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>150</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>186</v>
       </c>
-      <c r="D8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="H8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>99</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>151</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>187</v>
       </c>
-      <c r="D9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="H9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>100</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>152</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>188</v>
       </c>
-      <c r="D10" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>153</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>189</v>
       </c>
-      <c r="D11" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="H11" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>102</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>154</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>190</v>
       </c>
-      <c r="D12" t="s">
-        <v>143</v>
-      </c>
-      <c r="E12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="H12" t="s">
+        <v>143</v>
+      </c>
+      <c r="I12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>103</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>155</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>191</v>
       </c>
-      <c r="D13" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="H13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>104</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>156</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>192</v>
       </c>
-      <c r="D14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="H14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>157</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>193</v>
       </c>
-      <c r="D15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="H15" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>106</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>158</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>194</v>
       </c>
-      <c r="D16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="H16" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>107</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>159</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>195</v>
       </c>
-      <c r="D17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="H17" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>108</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>160</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>196</v>
       </c>
-      <c r="D18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>109</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>161</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>197</v>
       </c>
-      <c r="D19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="H19" t="s">
+        <v>143</v>
+      </c>
+      <c r="I19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>110</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>162</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>198</v>
       </c>
-      <c r="D20" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="H20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>111</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>163</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>199</v>
       </c>
-      <c r="D21" t="s">
-        <v>143</v>
-      </c>
-      <c r="E21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
+      <c r="I21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>112</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>164</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>200</v>
       </c>
-      <c r="D22" t="s">
-        <v>143</v>
-      </c>
-      <c r="E22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="H22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>113</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>165</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>201</v>
       </c>
-      <c r="D23" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="H23" t="s">
+        <v>143</v>
+      </c>
+      <c r="I23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>114</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>166</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>202</v>
       </c>
-      <c r="D24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="H24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>115</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>167</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>203</v>
       </c>
-      <c r="D25" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="H25" t="s">
+        <v>143</v>
+      </c>
+      <c r="I25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>129</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>168</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>204</v>
       </c>
-      <c r="D26" t="s">
-        <v>143</v>
-      </c>
-      <c r="E26" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="H26" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>128</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>169</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>205</v>
       </c>
-      <c r="D27" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="H27" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>116</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>170</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>206</v>
       </c>
-      <c r="D28" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="H28" t="s">
+        <v>143</v>
+      </c>
+      <c r="I28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>117</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>171</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>207</v>
       </c>
-      <c r="D29" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="H29" t="s">
+        <v>143</v>
+      </c>
+      <c r="I29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>118</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>172</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>208</v>
       </c>
-      <c r="D30" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="H30" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>119</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>173</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>209</v>
       </c>
-      <c r="D31" t="s">
-        <v>143</v>
-      </c>
-      <c r="E31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="H31" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>120</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>174</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>210</v>
       </c>
-      <c r="D32" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="H32" t="s">
+        <v>143</v>
+      </c>
+      <c r="I32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>121</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>175</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>211</v>
       </c>
-      <c r="D33" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="H33" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>122</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>176</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>212</v>
       </c>
-      <c r="D34" t="s">
-        <v>143</v>
-      </c>
-      <c r="E34" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="H34" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>123</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>177</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>213</v>
       </c>
-      <c r="D35" t="s">
-        <v>143</v>
-      </c>
-      <c r="E35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="H35" t="s">
+        <v>143</v>
+      </c>
+      <c r="I35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>124</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>178</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>214</v>
       </c>
-      <c r="D36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="H36" t="s">
+        <v>143</v>
+      </c>
+      <c r="I36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>125</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>179</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>215</v>
       </c>
-      <c r="D37" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="H37" t="s">
+        <v>143</v>
+      </c>
+      <c r="I37" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E37">
+  <autoFilter ref="A1:I37">
     <sortState ref="A2:E38">
       <sortCondition ref="A4"/>
     </sortState>
@@ -2421,7 +2449,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Merged data files into one Excel
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -12,7 +12,7 @@
     <sheet name="problems" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicators!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">indicators!$A$1:$F$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">municipalities!$A$1:$C$41</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="353">
   <si>
     <t>albanian</t>
   </si>
@@ -784,14 +784,321 @@
     <t>serbian_short</t>
   </si>
   <si>
-    <t>english_desc</t>
+    <t>Preschool education</t>
+  </si>
+  <si>
+    <t>Cemetery maintenance</t>
+  </si>
+  <si>
+    <t>Cultural activities</t>
+  </si>
+  <si>
+    <t>Electricity supply</t>
+  </si>
+  <si>
+    <t>Environmental protection</t>
+  </si>
+  <si>
+    <t>Family medical centers</t>
+  </si>
+  <si>
+    <t>Emergency services</t>
+  </si>
+  <si>
+    <t>Hospitals</t>
+  </si>
+  <si>
+    <t>Local road maintenance</t>
+  </si>
+  <si>
+    <t>Inter-municipal roads</t>
+  </si>
+  <si>
+    <t>Municipal funds</t>
+  </si>
+  <si>
+    <t>Municipal Administration</t>
+  </si>
+  <si>
+    <t>Municipal Assembly</t>
+  </si>
+  <si>
+    <t>Parks &amp; squares</t>
+  </si>
+  <si>
+    <t>Nature conservation</t>
+  </si>
+  <si>
+    <t>Postal services</t>
+  </si>
+  <si>
+    <t>Primary &amp; secondary education</t>
+  </si>
+  <si>
+    <t>Tax payment procedures</t>
+  </si>
+  <si>
+    <t>Cultural heritage</t>
+  </si>
+  <si>
+    <t>Public health</t>
+  </si>
+  <si>
+    <t>Public lighting</t>
+  </si>
+  <si>
+    <t>Public procurement</t>
+  </si>
+  <si>
+    <t>Public transport</t>
+  </si>
+  <si>
+    <t>Local staff</t>
+  </si>
+  <si>
+    <t>Ethnic minorities</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Sewage &amp; sanitation</t>
+  </si>
+  <si>
+    <t>Sidewalks</t>
+  </si>
+  <si>
+    <t>Social services</t>
+  </si>
+  <si>
+    <t>Sports activities</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t>Traffic &amp; parking</t>
+  </si>
+  <si>
+    <t>Urban &amp; rural planning</t>
+  </si>
+  <si>
+    <t>Waste collection</t>
+  </si>
+  <si>
+    <t>Water supply</t>
+  </si>
+  <si>
+    <t>Youth activities</t>
+  </si>
+  <si>
+    <t>Arsimimi parashkollor</t>
+  </si>
+  <si>
+    <t>Mirëmbajtja e varrezave</t>
+  </si>
+  <si>
+    <t>Furnizimi me rrymë</t>
+  </si>
+  <si>
+    <t>Mbrojtja e mjedisit</t>
+  </si>
+  <si>
+    <t>Shërbimet e emergjencës</t>
+  </si>
+  <si>
+    <t>Rrugët komunale</t>
+  </si>
+  <si>
+    <t>Rrugët ndërkomunale</t>
+  </si>
+  <si>
+    <t>Fondet komunale</t>
+  </si>
+  <si>
+    <t>Administrata komunale</t>
+  </si>
+  <si>
+    <t>Asambleja komunale</t>
+  </si>
+  <si>
+    <t>Parqet &amp; sheshet</t>
+  </si>
+  <si>
+    <t>Mbrojtja e natyrës</t>
+  </si>
+  <si>
+    <t>Shërbimet postare</t>
+  </si>
+  <si>
+    <t>Arsimimi fillor &amp; i mesëm</t>
+  </si>
+  <si>
+    <t>Pagesa e taksave</t>
+  </si>
+  <si>
+    <t>Trashëgimia kulturore</t>
+  </si>
+  <si>
+    <t>Shëndetësia publike</t>
+  </si>
+  <si>
+    <t>Ndriçimi publik</t>
+  </si>
+  <si>
+    <t>Prokurimi publik</t>
+  </si>
+  <si>
+    <t>Transporti publik</t>
+  </si>
+  <si>
+    <t>Stafi komunal</t>
+  </si>
+  <si>
+    <t>Pakicat etnike</t>
+  </si>
+  <si>
+    <t>Gratë</t>
+  </si>
+  <si>
+    <t>Kanalizimi</t>
+  </si>
+  <si>
+    <t>Kryetari/ja i/e komunës</t>
+  </si>
+  <si>
+    <t>Trafiku &amp; parkingu</t>
+  </si>
+  <si>
+    <t>Planifikimi urban &amp; rural</t>
+  </si>
+  <si>
+    <t>Mbledhja e mbeturinave</t>
+  </si>
+  <si>
+    <t>Aktivitetet rinore</t>
+  </si>
+  <si>
+    <t>Predškolsko obrazovanje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Održavanje groblja </t>
+  </si>
+  <si>
+    <t>Kulturne aktivnosti</t>
+  </si>
+  <si>
+    <t>Električna energija</t>
+  </si>
+  <si>
+    <t>Zaštita životne sredine</t>
+  </si>
+  <si>
+    <t>Porodičnim medicinskim centri</t>
+  </si>
+  <si>
+    <t>Hitna služba</t>
+  </si>
+  <si>
+    <t>Bolnice</t>
+  </si>
+  <si>
+    <t>Lokalni putevi</t>
+  </si>
+  <si>
+    <t>Međuopštinski putevi</t>
+  </si>
+  <si>
+    <t>Opštinski fondovi</t>
+  </si>
+  <si>
+    <t>Opštinska administracija</t>
+  </si>
+  <si>
+    <t>Opštinska skupština</t>
+  </si>
+  <si>
+    <t>Parkovi &amp; trgovi</t>
+  </si>
+  <si>
+    <t>Očuvanje prirode</t>
+  </si>
+  <si>
+    <t>Poštanske usluge</t>
+  </si>
+  <si>
+    <t>Osnovnog &amp; srednjo obrazovanje</t>
+  </si>
+  <si>
+    <t>Plaćanje poreza</t>
+  </si>
+  <si>
+    <t>Kulturno nasleđe</t>
+  </si>
+  <si>
+    <t>Javno zdravstvo</t>
+  </si>
+  <si>
+    <t>Javni rasvet</t>
+  </si>
+  <si>
+    <t>Javne nabavke</t>
+  </si>
+  <si>
+    <t>Javni prevoz</t>
+  </si>
+  <si>
+    <t>Opštinsko osoblje</t>
+  </si>
+  <si>
+    <t>Etničke manjine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> žene</t>
+  </si>
+  <si>
+    <t>Kanalizacija</t>
+  </si>
+  <si>
+    <t>Trotoari</t>
+  </si>
+  <si>
+    <t>Socijalne usluge</t>
+  </si>
+  <si>
+    <t>Sportske aktivnosti</t>
+  </si>
+  <si>
+    <t>Gradonačelnik/ca</t>
+  </si>
+  <si>
+    <t>Saobraćaj &amp; parking</t>
+  </si>
+  <si>
+    <t>Ruralno &amp; urbano planiranje</t>
+  </si>
+  <si>
+    <t>Prikupljanje otpada</t>
+  </si>
+  <si>
+    <t>Vodosnabdevanje</t>
+  </si>
+  <si>
+    <t>Omladinske aktivnosti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -835,66 +1142,66 @@
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -902,6 +1209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1768,10 +2076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1782,12 +2090,9 @@
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="55.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -1806,634 +2111,728 @@
       <c r="F1" t="s">
         <v>251</v>
       </c>
-      <c r="G1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>94</v>
       </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
       <c r="C2" t="s">
         <v>144</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>288</v>
+      </c>
       <c r="E2" t="s">
         <v>180</v>
       </c>
-      <c r="H2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="F2" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>127</v>
       </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
       <c r="C3" t="s">
         <v>145</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>289</v>
+      </c>
       <c r="E3" t="s">
         <v>181</v>
       </c>
-      <c r="H3" t="s">
-        <v>143</v>
-      </c>
-      <c r="I3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="F3" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>95</v>
       </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
       <c r="C4" t="s">
         <v>146</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="E4" t="s">
         <v>182</v>
       </c>
-      <c r="H4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="F4" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>96</v>
       </c>
+      <c r="B5" t="s">
+        <v>255</v>
+      </c>
       <c r="C5" t="s">
         <v>147</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="E5" t="s">
         <v>183</v>
       </c>
-      <c r="H5" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="F5" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>97</v>
       </c>
+      <c r="B6" t="s">
+        <v>256</v>
+      </c>
       <c r="C6" t="s">
         <v>148</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>291</v>
+      </c>
       <c r="E6" t="s">
         <v>184</v>
       </c>
-      <c r="H6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="F6" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>98</v>
       </c>
+      <c r="B7" t="s">
+        <v>257</v>
+      </c>
       <c r="C7" t="s">
         <v>149</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="E7" t="s">
         <v>185</v>
       </c>
-      <c r="H7" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="F7" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>130</v>
       </c>
+      <c r="B8" t="s">
+        <v>258</v>
+      </c>
       <c r="C8" t="s">
         <v>150</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="E8" t="s">
         <v>186</v>
       </c>
-      <c r="H8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="F8" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>99</v>
       </c>
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
       <c r="C9" t="s">
         <v>151</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="E9" t="s">
         <v>187</v>
       </c>
-      <c r="H9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="F9" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>100</v>
       </c>
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
       <c r="C10" t="s">
         <v>152</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>293</v>
+      </c>
       <c r="E10" t="s">
         <v>188</v>
       </c>
-      <c r="H10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="F10" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>101</v>
       </c>
+      <c r="B11" t="s">
+        <v>261</v>
+      </c>
       <c r="C11" t="s">
         <v>153</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>294</v>
+      </c>
       <c r="E11" t="s">
         <v>189</v>
       </c>
-      <c r="H11" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="F11" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>102</v>
       </c>
+      <c r="B12" t="s">
+        <v>262</v>
+      </c>
       <c r="C12" t="s">
         <v>154</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>295</v>
+      </c>
       <c r="E12" t="s">
         <v>190</v>
       </c>
-      <c r="H12" t="s">
-        <v>143</v>
-      </c>
-      <c r="I12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="F12" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>103</v>
       </c>
+      <c r="B13" t="s">
+        <v>263</v>
+      </c>
       <c r="C13" t="s">
         <v>155</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>296</v>
+      </c>
       <c r="E13" t="s">
         <v>191</v>
       </c>
-      <c r="H13" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="F13" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>104</v>
       </c>
+      <c r="B14" t="s">
+        <v>264</v>
+      </c>
       <c r="C14" t="s">
         <v>156</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>297</v>
+      </c>
       <c r="E14" t="s">
         <v>192</v>
       </c>
-      <c r="H14" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="F14" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>105</v>
       </c>
+      <c r="B15" t="s">
+        <v>265</v>
+      </c>
       <c r="C15" t="s">
         <v>157</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>298</v>
+      </c>
       <c r="E15" t="s">
         <v>193</v>
       </c>
-      <c r="H15" t="s">
-        <v>143</v>
-      </c>
-      <c r="I15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="F15" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>106</v>
       </c>
+      <c r="B16" t="s">
+        <v>266</v>
+      </c>
       <c r="C16" t="s">
         <v>158</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>299</v>
+      </c>
       <c r="E16" t="s">
         <v>194</v>
       </c>
-      <c r="H16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="F16" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>107</v>
       </c>
+      <c r="B17" t="s">
+        <v>267</v>
+      </c>
       <c r="C17" t="s">
         <v>159</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>300</v>
+      </c>
       <c r="E17" t="s">
         <v>195</v>
       </c>
-      <c r="H17" t="s">
-        <v>143</v>
-      </c>
-      <c r="I17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="F17" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>108</v>
       </c>
+      <c r="B18" t="s">
+        <v>268</v>
+      </c>
       <c r="C18" t="s">
         <v>160</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>301</v>
+      </c>
       <c r="E18" t="s">
         <v>196</v>
       </c>
-      <c r="H18" t="s">
-        <v>143</v>
-      </c>
-      <c r="I18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="F18" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>109</v>
       </c>
+      <c r="B19" t="s">
+        <v>269</v>
+      </c>
       <c r="C19" t="s">
         <v>161</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>302</v>
+      </c>
       <c r="E19" t="s">
         <v>197</v>
       </c>
-      <c r="H19" t="s">
-        <v>143</v>
-      </c>
-      <c r="I19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="F19" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>110</v>
       </c>
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
       <c r="C20" t="s">
         <v>162</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="E20" t="s">
         <v>198</v>
       </c>
-      <c r="H20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="F20" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>111</v>
       </c>
+      <c r="B21" t="s">
+        <v>271</v>
+      </c>
       <c r="C21" t="s">
         <v>163</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>304</v>
+      </c>
       <c r="E21" t="s">
         <v>199</v>
       </c>
-      <c r="H21" t="s">
-        <v>143</v>
-      </c>
-      <c r="I21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="F21" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>112</v>
       </c>
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
       <c r="C22" t="s">
         <v>164</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>305</v>
+      </c>
       <c r="E22" t="s">
         <v>200</v>
       </c>
-      <c r="H22" t="s">
-        <v>143</v>
-      </c>
-      <c r="I22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="F22" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>113</v>
       </c>
+      <c r="B23" t="s">
+        <v>273</v>
+      </c>
       <c r="C23" t="s">
         <v>165</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>306</v>
+      </c>
       <c r="E23" t="s">
         <v>201</v>
       </c>
-      <c r="H23" t="s">
-        <v>143</v>
-      </c>
-      <c r="I23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="F23" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>114</v>
       </c>
+      <c r="B24" t="s">
+        <v>274</v>
+      </c>
       <c r="C24" t="s">
         <v>166</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>307</v>
+      </c>
       <c r="E24" t="s">
         <v>202</v>
       </c>
-      <c r="H24" t="s">
-        <v>143</v>
-      </c>
-      <c r="I24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="F24" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>115</v>
       </c>
+      <c r="B25" t="s">
+        <v>275</v>
+      </c>
       <c r="C25" t="s">
         <v>167</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>308</v>
+      </c>
       <c r="E25" t="s">
         <v>203</v>
       </c>
-      <c r="H25" t="s">
-        <v>143</v>
-      </c>
-      <c r="I25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="F25" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>129</v>
       </c>
+      <c r="B26" t="s">
+        <v>276</v>
+      </c>
       <c r="C26" t="s">
         <v>168</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>309</v>
+      </c>
       <c r="E26" t="s">
         <v>204</v>
       </c>
-      <c r="H26" t="s">
-        <v>143</v>
-      </c>
-      <c r="I26" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="F26" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>128</v>
       </c>
+      <c r="B27" t="s">
+        <v>277</v>
+      </c>
       <c r="C27" t="s">
         <v>169</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>310</v>
+      </c>
       <c r="E27" t="s">
         <v>205</v>
       </c>
-      <c r="H27" t="s">
-        <v>143</v>
-      </c>
-      <c r="I27" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="F27" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>116</v>
       </c>
+      <c r="B28" t="s">
+        <v>278</v>
+      </c>
       <c r="C28" t="s">
         <v>170</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="E28" t="s">
         <v>206</v>
       </c>
-      <c r="H28" t="s">
-        <v>143</v>
-      </c>
-      <c r="I28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="F28" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>117</v>
       </c>
+      <c r="B29" t="s">
+        <v>279</v>
+      </c>
       <c r="C29" t="s">
         <v>171</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="E29" t="s">
         <v>207</v>
       </c>
-      <c r="H29" t="s">
-        <v>143</v>
-      </c>
-      <c r="I29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="F29" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>118</v>
       </c>
+      <c r="B30" t="s">
+        <v>280</v>
+      </c>
       <c r="C30" t="s">
         <v>172</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="E30" t="s">
         <v>208</v>
       </c>
-      <c r="H30" t="s">
-        <v>143</v>
-      </c>
-      <c r="I30" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="F30" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>119</v>
       </c>
+      <c r="B31" t="s">
+        <v>281</v>
+      </c>
       <c r="C31" t="s">
         <v>173</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="E31" t="s">
         <v>209</v>
       </c>
-      <c r="H31" t="s">
-        <v>143</v>
-      </c>
-      <c r="I31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="F31" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>120</v>
       </c>
+      <c r="B32" t="s">
+        <v>282</v>
+      </c>
       <c r="C32" t="s">
         <v>174</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>312</v>
+      </c>
       <c r="E32" t="s">
         <v>210</v>
       </c>
-      <c r="H32" t="s">
-        <v>143</v>
-      </c>
-      <c r="I32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="F32" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>121</v>
       </c>
+      <c r="B33" t="s">
+        <v>283</v>
+      </c>
       <c r="C33" t="s">
         <v>175</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="E33" t="s">
         <v>211</v>
       </c>
-      <c r="H33" t="s">
-        <v>143</v>
-      </c>
-      <c r="I33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="F33" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>122</v>
       </c>
+      <c r="B34" t="s">
+        <v>284</v>
+      </c>
       <c r="C34" t="s">
         <v>176</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>314</v>
+      </c>
       <c r="E34" t="s">
         <v>212</v>
       </c>
-      <c r="H34" t="s">
-        <v>143</v>
-      </c>
-      <c r="I34" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="F34" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>123</v>
       </c>
+      <c r="B35" t="s">
+        <v>285</v>
+      </c>
       <c r="C35" t="s">
         <v>177</v>
       </c>
+      <c r="D35" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="E35" t="s">
         <v>213</v>
       </c>
-      <c r="H35" t="s">
-        <v>143</v>
-      </c>
-      <c r="I35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="F35" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>124</v>
       </c>
+      <c r="B36" t="s">
+        <v>286</v>
+      </c>
       <c r="C36" t="s">
         <v>178</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="E36" t="s">
         <v>214</v>
       </c>
-      <c r="H36" t="s">
-        <v>143</v>
-      </c>
-      <c r="I36" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="F36" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>125</v>
       </c>
+      <c r="B37" t="s">
+        <v>287</v>
+      </c>
       <c r="C37" t="s">
         <v>179</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>316</v>
+      </c>
       <c r="E37" t="s">
         <v>215</v>
       </c>
-      <c r="H37" t="s">
-        <v>143</v>
-      </c>
-      <c r="I37" t="s">
-        <v>143</v>
+      <c r="F37" s="3" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I37">
-    <sortState ref="A2:E38">
-      <sortCondition ref="A4"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Fixing translation error in indicators whitelist
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="352">
   <si>
     <t>albanian</t>
   </si>
@@ -469,9 +469,6 @@
   </si>
   <si>
     <t>Furnizimin me energji elektrike</t>
-  </si>
-  <si>
-    <t>Aktivitetet e emergjencës</t>
   </si>
   <si>
     <t>Mbrojtjen e mjedisit</t>
@@ -1691,7 +1688,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1763,7 +1760,7 @@
         <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1859,10 +1856,10 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2079,7 +2076,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2097,19 +2094,19 @@
         <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2117,19 +2114,19 @@
         <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" t="s">
         <v>144</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2137,19 +2134,19 @@
         <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
         <v>145</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2157,7 +2154,7 @@
         <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C4" t="s">
         <v>146</v>
@@ -2166,10 +2163,10 @@
         <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2177,19 +2174,19 @@
         <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C5" t="s">
         <v>147</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2197,19 +2194,19 @@
         <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C6" t="s">
         <v>148</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2217,19 +2214,19 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C7" t="s">
         <v>149</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2237,19 +2234,19 @@
         <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>291</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2257,19 +2254,19 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2277,19 +2274,19 @@
         <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2297,19 +2294,19 @@
         <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2317,19 +2314,19 @@
         <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2337,19 +2334,19 @@
         <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2357,19 +2354,19 @@
         <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2377,19 +2374,19 @@
         <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2397,19 +2394,19 @@
         <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2417,19 +2414,19 @@
         <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2437,19 +2434,19 @@
         <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2457,19 +2454,19 @@
         <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2477,19 +2474,19 @@
         <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2497,19 +2494,19 @@
         <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2517,19 +2514,19 @@
         <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2537,19 +2534,19 @@
         <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2557,19 +2554,19 @@
         <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2577,19 +2574,19 @@
         <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2597,19 +2594,19 @@
         <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2617,19 +2614,19 @@
         <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2637,19 +2634,19 @@
         <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2657,19 +2654,19 @@
         <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2677,19 +2674,19 @@
         <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2697,19 +2694,19 @@
         <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2717,19 +2714,19 @@
         <v>120</v>
       </c>
       <c r="B32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2737,19 +2734,19 @@
         <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2757,19 +2754,19 @@
         <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2777,19 +2774,19 @@
         <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2797,19 +2794,19 @@
         <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2817,19 +2814,19 @@
         <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2871,10 +2868,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
         <v>243</v>
-      </c>
-      <c r="E1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2882,10 +2879,10 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D2" t="s">
         <v>143</v>
@@ -2899,10 +2896,10 @@
         <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" t="s">
         <v>143</v>
@@ -2916,10 +2913,10 @@
         <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
         <v>143</v>
@@ -2933,10 +2930,10 @@
         <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" t="s">
         <v>143</v>
@@ -2950,10 +2947,10 @@
         <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" t="s">
         <v>143</v>
@@ -2967,10 +2964,10 @@
         <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D7" t="s">
         <v>143</v>
@@ -2984,10 +2981,10 @@
         <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D8" t="s">
         <v>143</v>
@@ -3001,10 +2998,10 @@
         <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
         <v>143</v>
@@ -3018,10 +3015,10 @@
         <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" t="s">
         <v>143</v>
@@ -3035,10 +3032,10 @@
         <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D11" t="s">
         <v>143</v>
@@ -3049,13 +3046,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D12" t="s">
         <v>143</v>
@@ -3069,10 +3066,10 @@
         <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D13" t="s">
         <v>143</v>
@@ -3086,10 +3083,10 @@
         <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" t="s">
         <v>143</v>

</xml_diff>

<commit_message>
capitalized first letter of indicators and problems translation for english
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="municipalities" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="384">
   <si>
     <t>index</t>
   </si>
@@ -338,6 +338,9 @@
     <t>access to and quality of preschool education</t>
   </si>
   <si>
+    <t>Access to and quality of preschool education</t>
+  </si>
+  <si>
     <t>Preschool education</t>
   </si>
   <si>
@@ -488,6 +491,9 @@
     <t>maintenance of inter-municipal roads and highways</t>
   </si>
   <si>
+    <t>Maintenance of inter-municipal roads and highways</t>
+  </si>
+  <si>
     <t>Inter-municipal roads</t>
   </si>
   <si>
@@ -506,6 +512,9 @@
     <t>management of municipal funds</t>
   </si>
   <si>
+    <t>Management of municipal funds</t>
+  </si>
+  <si>
     <t>Municipal funds</t>
   </si>
   <si>
@@ -524,6 +533,9 @@
     <t>municipal administration</t>
   </si>
   <si>
+    <t>Municipal administration</t>
+  </si>
+  <si>
     <t>Municipal Administration</t>
   </si>
   <si>
@@ -542,6 +554,9 @@
     <t>municipal assembly</t>
   </si>
   <si>
+    <t>Municipal assembly</t>
+  </si>
+  <si>
     <t>Municipal Assembly</t>
   </si>
   <si>
@@ -560,6 +575,9 @@
     <t>municipal parks and squares</t>
   </si>
   <si>
+    <t>Municipal parks and squares</t>
+  </si>
+  <si>
     <t>Parks &amp; squares</t>
   </si>
   <si>
@@ -578,6 +596,9 @@
     <t>nature and species conservation</t>
   </si>
   <si>
+    <t>Nature and species conservation</t>
+  </si>
+  <si>
     <t>Nature conservation</t>
   </si>
   <si>
@@ -596,6 +617,9 @@
     <t>phone and postal services</t>
   </si>
   <si>
+    <t>Phone and postal services</t>
+  </si>
+  <si>
     <t>Postal services</t>
   </si>
   <si>
@@ -614,6 +638,9 @@
     <t>primary and secondary schools/education</t>
   </si>
   <si>
+    <t>Primary and secondary schools/education</t>
+  </si>
+  <si>
     <t>Primary &amp; secondary education</t>
   </si>
   <si>
@@ -632,6 +659,9 @@
     <t>procedures for tax payment</t>
   </si>
   <si>
+    <t>Procedures for tax payment</t>
+  </si>
+  <si>
     <t>Tax payment procedures</t>
   </si>
   <si>
@@ -650,6 +680,9 @@
     <t>protection of cultural heritage</t>
   </si>
   <si>
+    <t>Protection of cultural heritage</t>
+  </si>
+  <si>
     <t>Cultural heritage</t>
   </si>
   <si>
@@ -704,6 +737,9 @@
     <t>public procurement/tenders</t>
   </si>
   <si>
+    <t>Public procurement/tenders</t>
+  </si>
+  <si>
     <t>Public procurement</t>
   </si>
   <si>
@@ -740,6 +776,9 @@
     <t>recruitment of local staff</t>
   </si>
   <si>
+    <t>Recruitment of local staff</t>
+  </si>
+  <si>
     <t>Local staff</t>
   </si>
   <si>
@@ -758,6 +797,9 @@
     <t>representation of ethnic minorities</t>
   </si>
   <si>
+    <t>Representation of ethnic minorities</t>
+  </si>
+  <si>
     <t>Ethnic minorities</t>
   </si>
   <si>
@@ -776,6 +818,9 @@
     <t>representation of women</t>
   </si>
   <si>
+    <t>Representation of women</t>
+  </si>
+  <si>
     <t>Women</t>
   </si>
   <si>
@@ -794,6 +839,9 @@
     <t>sewage and sanitation</t>
   </si>
   <si>
+    <t>Sewage and sanitation</t>
+  </si>
+  <si>
     <t>Sewage &amp; sanitation</t>
   </si>
   <si>
@@ -857,6 +905,9 @@
     <t>the mayor</t>
   </si>
   <si>
+    <t>The mayor</t>
+  </si>
+  <si>
     <t>Mayor</t>
   </si>
   <si>
@@ -875,6 +926,9 @@
     <t>traffic and parking control and regulation</t>
   </si>
   <si>
+    <t>Traffic and parking control and regulation</t>
+  </si>
+  <si>
     <t>Traffic &amp; parking</t>
   </si>
   <si>
@@ -893,6 +947,9 @@
     <t>urban and rural planning</t>
   </si>
   <si>
+    <t>Urban and rural planning</t>
+  </si>
+  <si>
     <t>Urban &amp; rural planning</t>
   </si>
   <si>
@@ -911,6 +968,9 @@
     <t>waste collection services</t>
   </si>
   <si>
+    <t>Waste collection services</t>
+  </si>
+  <si>
     <t>Waste collection</t>
   </si>
   <si>
@@ -965,6 +1025,9 @@
     <t>corruption</t>
   </si>
   <si>
+    <t>Corruption</t>
+  </si>
+  <si>
     <t>Korrupsioni</t>
   </si>
   <si>
@@ -974,6 +1037,9 @@
     <t>crime</t>
   </si>
   <si>
+    <t>Crime</t>
+  </si>
+  <si>
     <t>Krimi</t>
   </si>
   <si>
@@ -983,6 +1049,9 @@
     <t>environmental pollution</t>
   </si>
   <si>
+    <t>Environmental pollution</t>
+  </si>
+  <si>
     <t>Ndotja e mjedisit</t>
   </si>
   <si>
@@ -992,6 +1061,9 @@
     <t>inter-ethnic relations</t>
   </si>
   <si>
+    <t>Inter-ethnic relations</t>
+  </si>
+  <si>
     <t>Marrëdhëniet ndërt-etnike</t>
   </si>
   <si>
@@ -1001,6 +1073,9 @@
     <t>lack of economic growth</t>
   </si>
   <si>
+    <t>Lack of economic growth</t>
+  </si>
+  <si>
     <t>Mungesa e rritjes ekonomike</t>
   </si>
   <si>
@@ -1010,6 +1085,9 @@
     <t>lack of general or personal security</t>
   </si>
   <si>
+    <t>Lack of general or personal security</t>
+  </si>
+  <si>
     <t>Mungesa e sigurisë së përgjithshme dhe sigurisë personale</t>
   </si>
   <si>
@@ -1019,6 +1097,9 @@
     <t>limited freedom of movement</t>
   </si>
   <si>
+    <t>Limited freedom of movement</t>
+  </si>
+  <si>
     <t>Liria e kufizuar e lëvizjes</t>
   </si>
   <si>
@@ -1028,6 +1109,9 @@
     <t>poor electricity supply</t>
   </si>
   <si>
+    <t>Poor electricity supply</t>
+  </si>
+  <si>
     <t>Furnizimi me rryme</t>
   </si>
   <si>
@@ -1037,12 +1121,18 @@
     <t>poor water supply</t>
   </si>
   <si>
+    <t>Poor water supply</t>
+  </si>
+  <si>
     <t>Loše snabdevanje vodom</t>
   </si>
   <si>
     <t>poorly functioning rubbish collection service</t>
   </si>
   <si>
+    <t>Poorly functioning rubbish collection service</t>
+  </si>
+  <si>
     <t>Shërbimi i grumbullimit të mbeturinave</t>
   </si>
   <si>
@@ -1052,6 +1142,9 @@
     <t>poverty/low standard of living</t>
   </si>
   <si>
+    <t>Poverty/low standard of living</t>
+  </si>
+  <si>
     <t>Varfëria/Standardi i ulët i jetesës</t>
   </si>
   <si>
@@ -1061,6 +1154,9 @@
     <t>road infrastructure</t>
   </si>
   <si>
+    <t>Road infrastructure</t>
+  </si>
+  <si>
     <t>Infrastruktura rrugore</t>
   </si>
   <si>
@@ -1068,6 +1164,9 @@
   </si>
   <si>
     <t>unemployment</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
   </si>
   <si>
     <t>Papunësia</t>
@@ -1185,8 +1284,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1790,7 +1889,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D2:D41 B2"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1832,827 +1931,827 @@
         <v>104</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2673,8 +2772,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D2:D41 B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2701,184 +2800,184 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>315</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>316</v>
+        <v>337</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>316</v>
+        <v>338</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>322</v>
+        <v>345</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>322</v>
+        <v>346</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>324</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>325</v>
+        <v>349</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>328</v>
+        <v>353</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>330</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>333</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>334</v>
+        <v>361</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>335</v>
+        <v>363</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>336</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>337</v>
+        <v>365</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>337</v>
+        <v>366</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>338</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>339</v>
+        <v>368</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>339</v>
+        <v>369</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>340</v>
+        <v>370</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>341</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>342</v>
+        <v>372</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>342</v>
+        <v>373</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>343</v>
+        <v>374</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>344</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>345</v>
+        <v>376</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>345</v>
+        <v>377</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>346</v>
+        <v>378</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>347</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>348</v>
+        <v>380</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>348</v>
+        <v>381</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>349</v>
+        <v>382</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small updates to indicator text in Albanian and Serbian
</commit_message>
<xml_diff>
--- a/data/standard_lists/whitelist.xlsx
+++ b/data/standard_lists/whitelist.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="municipalities" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="indicators" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="problems" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="municipalities" sheetId="1" r:id="rId1"/>
+    <sheet name="indicators" sheetId="2" r:id="rId2"/>
+    <sheet name="problems" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">municipalities!$A$1:$C$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">indicators!$A$1:$G$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">indicators!$A$1:$G$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">municipalities!$A$1:$C$41</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="360">
   <si>
     <t>index</t>
   </si>
@@ -344,15 +343,9 @@
     <t>Preschool education</t>
   </si>
   <si>
-    <t>Qasjen dhe cilësinë e arsimimit parashkollor</t>
-  </si>
-  <si>
     <t>Arsimimi parashkollor</t>
   </si>
   <si>
-    <t>Pristupom i kvalitetom predškolskog obrazovanja</t>
-  </si>
-  <si>
     <t>Predškolsko obrazovanje</t>
   </si>
   <si>
@@ -362,15 +355,9 @@
     <t>Cemetery maintenance</t>
   </si>
   <si>
-    <t>Mirëmbajtjen e varrezave</t>
-  </si>
-  <si>
     <t>Mirëmbajtja e varrezave</t>
   </si>
   <si>
-    <t>Održavanjem groblja</t>
-  </si>
-  <si>
     <t>Održavanje groblja</t>
   </si>
   <si>
@@ -383,9 +370,6 @@
     <t>Aktivitetet e kulturës</t>
   </si>
   <si>
-    <t>Kulturnim aktivnostima</t>
-  </si>
-  <si>
     <t>Kulturne aktivnosti</t>
   </si>
   <si>
@@ -395,15 +379,9 @@
     <t>Electricity supply</t>
   </si>
   <si>
-    <t>Furnizimin me energji elektrike</t>
-  </si>
-  <si>
     <t>Furnizimi me rrymë</t>
   </si>
   <si>
-    <t>Snabdevanjem električnom energijom</t>
-  </si>
-  <si>
     <t>Električna energija</t>
   </si>
   <si>
@@ -413,15 +391,9 @@
     <t>Environmental protection</t>
   </si>
   <si>
-    <t>Mbrojtjen e mjedisit</t>
-  </si>
-  <si>
     <t>Mbrojtja e mjedisit</t>
   </si>
   <si>
-    <t>Hitnim službama</t>
-  </si>
-  <si>
     <t>Hitna služba</t>
   </si>
   <si>
@@ -434,9 +406,6 @@
     <t>Qendrat e mjekësisë familjare</t>
   </si>
   <si>
-    <t>Zaštitom životne sredine</t>
-  </si>
-  <si>
     <t>Zaštita životne sredine</t>
   </si>
   <si>
@@ -452,12 +421,6 @@
     <t>Shërbimet e emergjencës</t>
   </si>
   <si>
-    <t>Porodičnim medicinskim centrima</t>
-  </si>
-  <si>
-    <t>Porodičnim medicinskim centri</t>
-  </si>
-  <si>
     <t>hospitals</t>
   </si>
   <si>
@@ -467,9 +430,6 @@
     <t>Spitalet</t>
   </si>
   <si>
-    <t>Bolnicama</t>
-  </si>
-  <si>
     <t>Bolnice</t>
   </si>
   <si>
@@ -479,15 +439,9 @@
     <t>Local road maintenance</t>
   </si>
   <si>
-    <t>Mirëmbajtjen e rrugëve komunale</t>
-  </si>
-  <si>
     <t>Rrugët komunale</t>
   </si>
   <si>
-    <t>Održavanjem lokalnih puteva</t>
-  </si>
-  <si>
     <t>Lokalni putevi</t>
   </si>
   <si>
@@ -500,15 +454,9 @@
     <t>Inter-municipal roads</t>
   </si>
   <si>
-    <t>Mirëmbajtjen e rrugëve dhe autostradave ndërkomunale</t>
-  </si>
-  <si>
     <t>Rrugët ndërkomunale</t>
   </si>
   <si>
-    <t>Pristupačnošću i održavanjem međuopštinskih puteva i autoputeva</t>
-  </si>
-  <si>
     <t>Međuopštinski putevi</t>
   </si>
   <si>
@@ -521,15 +469,9 @@
     <t>Municipal funds</t>
   </si>
   <si>
-    <t>Menaxhimin e fondeve komunale</t>
-  </si>
-  <si>
     <t>Fondet komunale</t>
   </si>
   <si>
-    <t>Upravljanjem opštinskih fondova</t>
-  </si>
-  <si>
     <t>Opštinski fondovi</t>
   </si>
   <si>
@@ -542,15 +484,9 @@
     <t>Municipal Administration</t>
   </si>
   <si>
-    <t>Administratën publike</t>
-  </si>
-  <si>
     <t>Administrata komunale</t>
   </si>
   <si>
-    <t>Opštinskom administracijom</t>
-  </si>
-  <si>
     <t>Opštinska administracija</t>
   </si>
   <si>
@@ -563,15 +499,9 @@
     <t>Municipal Assembly</t>
   </si>
   <si>
-    <t>Asamblenë komunale</t>
-  </si>
-  <si>
     <t>Asambleja komunale</t>
   </si>
   <si>
-    <t>Opštinskom skupštinom</t>
-  </si>
-  <si>
     <t>Opštinska skupština</t>
   </si>
   <si>
@@ -590,9 +520,6 @@
     <t>Parqet &amp; sheshet</t>
   </si>
   <si>
-    <t>Opštinskim parkova i trgova</t>
-  </si>
-  <si>
     <t>Parkovi &amp; trgovi</t>
   </si>
   <si>
@@ -605,15 +532,9 @@
     <t>Nature conservation</t>
   </si>
   <si>
-    <t>Mbrojtjen e natyrës dhe specieve</t>
-  </si>
-  <si>
     <t>Mbrojtja e natyrës</t>
   </si>
   <si>
-    <t>Očuvanjem prirode i vrsta</t>
-  </si>
-  <si>
     <t>Očuvanje prirode</t>
   </si>
   <si>
@@ -626,15 +547,9 @@
     <t>Postal services</t>
   </si>
   <si>
-    <t>Telefoninë dhe shërbimet postare</t>
-  </si>
-  <si>
     <t>Shërbimet postare</t>
   </si>
   <si>
-    <t>Telefonskim i poštanskim uslugama</t>
-  </si>
-  <si>
     <t>Poštanske usluge</t>
   </si>
   <si>
@@ -647,18 +562,9 @@
     <t>Primary &amp; secondary education</t>
   </si>
   <si>
-    <t>Arsimimin fillor dhe të mesëm</t>
-  </si>
-  <si>
     <t>Arsimimi fillor &amp; i mesëm</t>
   </si>
   <si>
-    <t>Pristupom i kvalitetom osnovnog i srednog obrazovanja</t>
-  </si>
-  <si>
-    <t>Osnovnog &amp; srednjo obrazovanje</t>
-  </si>
-  <si>
     <t>procedures for tax payment</t>
   </si>
   <si>
@@ -674,9 +580,6 @@
     <t>Pagesa e taksave</t>
   </si>
   <si>
-    <t>Procedurama za plaćanje poreza</t>
-  </si>
-  <si>
     <t>Plaćanje poreza</t>
   </si>
   <si>
@@ -689,15 +592,9 @@
     <t>Cultural heritage</t>
   </si>
   <si>
-    <t>Mbrojtjen e trashëgimisë kulturore</t>
-  </si>
-  <si>
     <t>Trashëgimia kulturore</t>
   </si>
   <si>
-    <t>Zaštitom kulturnog nasleđa</t>
-  </si>
-  <si>
     <t>Kulturno nasleđe</t>
   </si>
   <si>
@@ -707,15 +604,9 @@
     <t>Public health</t>
   </si>
   <si>
-    <t>Shëndetësine publike</t>
-  </si>
-  <si>
     <t>Shëndetësia publike</t>
   </si>
   <si>
-    <t>Javnom zdravstvom</t>
-  </si>
-  <si>
     <t>Javno zdravstvo</t>
   </si>
   <si>
@@ -725,15 +616,9 @@
     <t>Public lighting</t>
   </si>
   <si>
-    <t>Ndriçimin publik</t>
-  </si>
-  <si>
     <t>Ndriçimi publik</t>
   </si>
   <si>
-    <t>Javnom rasvetom</t>
-  </si>
-  <si>
     <t>Javni rasvet</t>
   </si>
   <si>
@@ -746,15 +631,9 @@
     <t>Public procurement</t>
   </si>
   <si>
-    <t>Prokurimin publik/tenderët</t>
-  </si>
-  <si>
     <t>Prokurimi publik</t>
   </si>
   <si>
-    <t>Javnim nabavkama i tenderima</t>
-  </si>
-  <si>
     <t>Javne nabavke</t>
   </si>
   <si>
@@ -764,15 +643,9 @@
     <t>Public transport</t>
   </si>
   <si>
-    <t>Transportin publik</t>
-  </si>
-  <si>
     <t>Transporti publik</t>
   </si>
   <si>
-    <t>Javnim prevozom</t>
-  </si>
-  <si>
     <t>Javni prevoz</t>
   </si>
   <si>
@@ -785,15 +658,9 @@
     <t>Local staff</t>
   </si>
   <si>
-    <t>Punësimin e stafit të komunës</t>
-  </si>
-  <si>
     <t>Stafi komunal</t>
   </si>
   <si>
-    <t>Regrutovanjem opštinskog osoblja</t>
-  </si>
-  <si>
     <t>Opštinsko osoblje</t>
   </si>
   <si>
@@ -806,9 +673,6 @@
     <t>Ethnic minorities</t>
   </si>
   <si>
-    <t>Përfaqësimin e minoriteteve entike në komunë</t>
-  </si>
-  <si>
     <t>Pakicat etnike</t>
   </si>
   <si>
@@ -827,9 +691,6 @@
     <t>Women</t>
   </si>
   <si>
-    <t>Përfaqësimin e grave në komunë</t>
-  </si>
-  <si>
     <t>Gratë</t>
   </si>
   <si>
@@ -848,15 +709,9 @@
     <t>Sewage &amp; sanitation</t>
   </si>
   <si>
-    <t>Sistemin e kanalizimit</t>
-  </si>
-  <si>
     <t>Kanalizimi</t>
   </si>
   <si>
-    <t>Kanalizacijom i sanitacijom</t>
-  </si>
-  <si>
     <t>Kanalizacija</t>
   </si>
   <si>
@@ -869,9 +724,6 @@
     <t>Trotuaret</t>
   </si>
   <si>
-    <t>Trotoarima</t>
-  </si>
-  <si>
     <t>Trotoari</t>
   </si>
   <si>
@@ -884,9 +736,6 @@
     <t>Shërbimet sociale</t>
   </si>
   <si>
-    <t>Radom centara za socijalni rad</t>
-  </si>
-  <si>
     <t>Socijalne usluge</t>
   </si>
   <si>
@@ -899,9 +748,6 @@
     <t>Aktivitetet e sportit</t>
   </si>
   <si>
-    <t>Sportskim aktivnostima</t>
-  </si>
-  <si>
     <t>Sportske aktivnosti</t>
   </si>
   <si>
@@ -914,15 +760,9 @@
     <t>Mayor</t>
   </si>
   <si>
-    <t>Kryetarin e komunës</t>
-  </si>
-  <si>
     <t>Kryetari/ja i/e komunës</t>
   </si>
   <si>
-    <t>Gradonačelnikom</t>
-  </si>
-  <si>
     <t>Gradonačelnik/ca</t>
   </si>
   <si>
@@ -935,15 +775,9 @@
     <t>Traffic &amp; parking</t>
   </si>
   <si>
-    <t>Kontrollin dhe rregullimin e trafikut dhe parkingjeve</t>
-  </si>
-  <si>
     <t>Trafiku &amp; parkingu</t>
   </si>
   <si>
-    <t>Kontrolom i regulacijom parkinga i saobraćaja</t>
-  </si>
-  <si>
     <t>Saobraćaj &amp; parking</t>
   </si>
   <si>
@@ -956,15 +790,9 @@
     <t>Urban &amp; rural planning</t>
   </si>
   <si>
-    <t>Planfikimin urban dhe rural</t>
-  </si>
-  <si>
     <t>Planifikimi urban &amp; rural</t>
   </si>
   <si>
-    <t>Ruralnim i urbanim planiranjem</t>
-  </si>
-  <si>
     <t>Ruralno &amp; urbano planiranje</t>
   </si>
   <si>
@@ -977,15 +805,9 @@
     <t>Waste collection</t>
   </si>
   <si>
-    <t>Shërbimin e mbledhjes së mbeturinave</t>
-  </si>
-  <si>
     <t>Mbledhja e mbeturinave</t>
   </si>
   <si>
-    <t>Prikupljanjem i odlaganjem čvrstog otpada</t>
-  </si>
-  <si>
     <t>Prikupljanje otpada</t>
   </si>
   <si>
@@ -995,15 +817,9 @@
     <t>Water supply</t>
   </si>
   <si>
-    <t>Furnizimin me ujë</t>
-  </si>
-  <si>
     <t>Furnizimi me ujë</t>
   </si>
   <si>
-    <t>Vodosnabdevanjem</t>
-  </si>
-  <si>
     <t>Vodosnabdevanje</t>
   </si>
   <si>
@@ -1019,9 +835,6 @@
     <t>Aktivitetet rinore</t>
   </si>
   <si>
-    <t>Omladinskim aktivnostima</t>
-  </si>
-  <si>
     <t>Omladinske aktivnosti</t>
   </si>
   <si>
@@ -1176,37 +989,130 @@
   </si>
   <si>
     <t>Nezaposlenost</t>
+  </si>
+  <si>
+    <t>Qasja dhe cilësia e arsimimit parashkollor</t>
+  </si>
+  <si>
+    <t>Furnizimi me energji elektrike</t>
+  </si>
+  <si>
+    <t>Mirëmbajtja e rrugëve komunale</t>
+  </si>
+  <si>
+    <t>Mirëmbajtja e rrugëve dhe autostradave ndërkomunale</t>
+  </si>
+  <si>
+    <t>Menaxhimi i fondeve komunale</t>
+  </si>
+  <si>
+    <t>Mbrojtja e natyrës dhe specieve</t>
+  </si>
+  <si>
+    <t>Telefonia dhe shërbimet postare</t>
+  </si>
+  <si>
+    <t>Arsimimi fillor dhe i mesëm</t>
+  </si>
+  <si>
+    <t>Mbrojtja e trashëgimisë kulturore</t>
+  </si>
+  <si>
+    <t>Prokurimi publik/tenderët</t>
+  </si>
+  <si>
+    <t>Punësimi i stafit të komunës</t>
+  </si>
+  <si>
+    <t>Përfaqësimi i minoriteteve entike në komunë</t>
+  </si>
+  <si>
+    <t>Përfaqësimi i grave në komunë</t>
+  </si>
+  <si>
+    <t>Sistemi i kanalizimit</t>
+  </si>
+  <si>
+    <t>Kontrolli dhe rregullimi i trafikut dhe parkingjeve</t>
+  </si>
+  <si>
+    <t>Planfikimi urban dhe rural</t>
+  </si>
+  <si>
+    <t>Shërbimi i mbledhjes së mbeturinave</t>
+  </si>
+  <si>
+    <t>Pristup i kvalitet predškolskog obrazovanja</t>
+  </si>
+  <si>
+    <t>Snabdevanje električnom energijom</t>
+  </si>
+  <si>
+    <t>Porodični medicinski centri</t>
+  </si>
+  <si>
+    <t>Održavanje lokalnih puteva</t>
+  </si>
+  <si>
+    <t>Pristupačnošća i održavanje međuopštinskih puteva i autoputeva</t>
+  </si>
+  <si>
+    <t>Upravljanje opštinskih fondova</t>
+  </si>
+  <si>
+    <t>Opštinski parkovi i trgovi</t>
+  </si>
+  <si>
+    <t>Očuvanje prirode i vrsta</t>
+  </si>
+  <si>
+    <t>Telefonske i poštanske usluge</t>
+  </si>
+  <si>
+    <t>Pristup i kvalitet osnovnog i srednog obrazovanja</t>
+  </si>
+  <si>
+    <t>Procedure za plaćanje poreza</t>
+  </si>
+  <si>
+    <t>Zaštita kulturnog nasleđa</t>
+  </si>
+  <si>
+    <t>Javne nabavke i tenderi</t>
+  </si>
+  <si>
+    <t>Regrutovanje opštinskog osoblja</t>
+  </si>
+  <si>
+    <t>Kanalizacija i sanitacija</t>
+  </si>
+  <si>
+    <t>Rad centara za socijalni rad</t>
+  </si>
+  <si>
+    <t>Kontrola i regulacija parkinga i saobraćaja</t>
+  </si>
+  <si>
+    <t>Ruralno i urbano planiranje</t>
+  </si>
+  <si>
+    <t>Prikupljanje i odlaganje čvrstog otpada</t>
+  </si>
+  <si>
+    <t>Osnovno &amp; srednjo obrazovanje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1218,7 +1124,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1226,1770 +1132,1996 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5296296296296"/>
+    <col min="1" max="1" width="26"/>
+    <col min="2" max="2" width="26.625"/>
+    <col min="3" max="3" width="25.5"/>
+    <col min="4" max="1025" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" t="s">
         <v>97</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.6592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="36.8333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.6592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.8296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.662962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5296296296296"/>
+    <col min="1" max="1" width="41.625"/>
+    <col min="2" max="3" width="36.875"/>
+    <col min="4" max="4" width="42.625"/>
+    <col min="5" max="5" width="25.375"/>
+    <col min="6" max="6" width="55.875"/>
+    <col min="7" max="7" width="49.625"/>
+    <col min="8" max="1025" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="0" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="E3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="0" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="G4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C5" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="F5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B6" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="B7" t="s">
         <v>126</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="E7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="G7" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="B8" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="C8" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="D8" t="s">
         <v>132</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" t="s">
+        <v>342</v>
+      </c>
+      <c r="G8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B9" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F9" t="s">
         <v>136</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F7" s="0" t="s">
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>137</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="B10" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>325</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="F10" t="s">
+        <v>343</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="0" t="s">
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="B11" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="C11" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="D11" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="F11" t="s">
+        <v>344</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="B12" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="C12" t="s">
         <v>148</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="D12" t="s">
+        <v>327</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="F12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="0" t="s">
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
         <v>151</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="0" t="s">
+      <c r="B13" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="C13" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="D13" t="s">
         <v>154</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="G13" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
         <v>156</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B14" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C14" t="s">
         <v>158</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D14" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" t="s">
         <v>160</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G14" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
         <v>161</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="B15" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="C15" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="D15" t="s">
         <v>164</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="F15" t="s">
+        <v>346</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E12" s="1" t="s">
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
         <v>167</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="B16" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="C16" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="D16" t="s">
+        <v>328</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="F16" t="s">
+        <v>347</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="0" t="s">
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="B17" t="s">
         <v>173</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="C17" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="D17" t="s">
+        <v>329</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="F17" t="s">
+        <v>348</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
         <v>177</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B18" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C18" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F18" t="s">
+        <v>349</v>
+      </c>
+      <c r="G18" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="B19" t="s">
         <v>182</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="C19" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="D19" t="s">
         <v>184</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="F19" t="s">
+        <v>350</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D15" s="0" t="s">
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
         <v>187</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="B20" t="s">
         <v>188</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="C20" t="s">
         <v>189</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="D20" t="s">
+        <v>331</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="F20" t="s">
+        <v>351</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B16" s="0" t="s">
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="B21" t="s">
         <v>193</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" t="s">
         <v>194</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E21" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F21" t="s">
         <v>195</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="G21" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
         <v>196</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="B22" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="C22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" t="s">
         <v>198</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="E22" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="G22" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
         <v>200</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="B23" t="s">
         <v>201</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="C23" t="s">
         <v>202</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="D23" t="s">
+        <v>332</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="F23" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B24" t="s">
         <v>206</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" t="s">
         <v>207</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E24" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" t="s">
         <v>208</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>209</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="B25" t="s">
         <v>210</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="C25" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="D25" t="s">
+        <v>333</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="F25" t="s">
+        <v>353</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C19" s="0" t="s">
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>214</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="B26" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="C26" t="s">
         <v>216</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="D26" t="s">
+        <v>334</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="F26" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="G26" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B20" s="0" t="s">
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
         <v>220</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="B27" t="s">
         <v>221</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="C27" t="s">
         <v>222</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="D27" t="s">
+        <v>335</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F27" t="s">
         <v>224</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
         <v>226</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B28" t="s">
         <v>227</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="C28" t="s">
         <v>228</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="D28" t="s">
+        <v>336</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F28" t="s">
+        <v>354</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G21" s="1" t="s">
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="B29" t="s">
         <v>232</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C29" t="s">
+        <v>232</v>
+      </c>
+      <c r="D29" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="F29" t="s">
         <v>234</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G29" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
         <v>235</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="B30" t="s">
         <v>236</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="C30" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="E30" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F30" t="s">
+        <v>355</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B23" s="0" t="s">
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
         <v>239</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="B31" t="s">
         <v>240</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="C31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D31" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F31" t="s">
         <v>242</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G31" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>243</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="B32" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="C32" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="D32" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="F32" t="s">
         <v>247</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G32" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
         <v>248</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="B33" t="s">
         <v>249</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="C33" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="D33" t="s">
+        <v>337</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="F33" t="s">
+        <v>356</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C25" s="0" t="s">
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
         <v>253</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="B34" t="s">
         <v>254</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="C34" t="s">
         <v>255</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="D34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="F34" t="s">
+        <v>357</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
         <v>258</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B35" t="s">
         <v>259</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C35" t="s">
         <v>260</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D35" t="s">
+        <v>339</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F35" t="s">
+        <v>358</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F26" s="0" t="s">
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
         <v>263</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="B36" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="C36" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" t="s">
         <v>265</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="E36" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F36" t="s">
         <v>266</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="G36" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
         <v>267</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="B37" t="s">
         <v>268</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="C37" t="s">
+        <v>268</v>
+      </c>
+      <c r="D37" t="s">
         <v>269</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="F37" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>332</v>
-      </c>
       <c r="G37" s="1" t="s">
-        <v>333</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.662962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="48.9962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5296296296296"/>
+    <col min="1" max="1" width="37.625"/>
+    <col min="2" max="3" width="49"/>
+    <col min="4" max="4" width="40"/>
+    <col min="5" max="1025" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>374</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>384</v>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" t="s">
+        <v>302</v>
+      </c>
+      <c r="D9" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" t="s">
+        <v>305</v>
+      </c>
+      <c r="C10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>307</v>
+      </c>
+      <c r="B11" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" t="s">
+        <v>309</v>
+      </c>
+      <c r="D11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B12" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" t="s">
+        <v>313</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>315</v>
+      </c>
+      <c r="B13" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" t="s">
+        <v>321</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>